<commit_message>
UPD all related with ImportModuleFromParallel_folder.py
</commit_message>
<xml_diff>
--- a/iggPyBlog-test_excersices_status.xlsx
+++ b/iggPyBlog-test_excersices_status.xlsx
@@ -423,7 +423,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -706,11 +706,11 @@
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>7</v>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6">

</xml_diff>